<commit_message>
update sprint planning based on first feedback
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Moeri\Google Drive\BFH\20FS\SEaD\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812D960D-5A53-491B-BA7E-236D60B72F95}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F32984-AEC9-42A7-9333-DDD3DC553D2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Navigation Component</t>
   </si>
   <si>
-    <t>Router</t>
-  </si>
-  <si>
     <t>Create a Test Set of at least 20 Appointments that cover different relationships</t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t>Display the upcoming appointments of a patient on his profile.</t>
   </si>
   <si>
-    <t>Set up a routing mechanism</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -420,6 +414,12 @@
   </si>
   <si>
     <t>View Patients</t>
+  </si>
+  <si>
+    <t>Navigation Architecture</t>
+  </si>
+  <si>
+    <t>Set up page skeletons and a routing mechanism</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -560,6 +560,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,7 +1297,7 @@
       </c>
       <c r="F2" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A2,'Sprint Backlog'!K:K)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A2,'Sprint Backlog'!L:L)</f>
@@ -1303,7 +1312,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>44</v>
@@ -1594,7 +1603,7 @@
   <dimension ref="A1:CA444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,10 +1741,12 @@
       <c r="E2" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H2" s="9"/>
       <c r="I2" s="11" t="s">
         <v>5</v>
@@ -1768,7 +1779,7 @@
       <c r="E3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="25" t="s">
         <v>97</v>
       </c>
       <c r="G3" s="13"/>
@@ -1806,7 +1817,7 @@
       <c r="E4" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="24" t="s">
         <v>98</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1817,10 +1828,10 @@
         <v>6</v>
       </c>
       <c r="J4" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11" t="s">
@@ -1844,7 +1855,7 @@
       <c r="E5" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="25" t="s">
         <v>99</v>
       </c>
       <c r="G5" s="13"/>
@@ -1882,7 +1893,7 @@
       <c r="E6" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="24" t="s">
         <v>81</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -1920,7 +1931,7 @@
       <c r="E7" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="25" t="s">
         <v>87</v>
       </c>
       <c r="G7" s="13"/>
@@ -1939,7 +1950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>1.7</v>
       </c>
@@ -1951,13 +1962,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>122</v>
+        <v>127</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -1992,8 +2003,8 @@
       <c r="E9" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>122</v>
+      <c r="F9" s="25" t="s">
+        <v>120</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -2028,7 +2039,7 @@
       <c r="E10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="24" t="s">
         <v>86</v>
       </c>
       <c r="G10" s="9"/>
@@ -2064,10 +2075,12 @@
       <c r="E11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="15" t="s">
         <v>5</v>
@@ -2100,7 +2113,7 @@
       <c r="E12" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="24" t="s">
         <v>96</v>
       </c>
       <c r="G12" s="9"/>
@@ -2138,7 +2151,7 @@
       <c r="E13" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="25" t="s">
         <v>95</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -2174,9 +2187,9 @@
         <v>72</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>90</v>
       </c>
       <c r="G14" s="9"/>
@@ -2210,9 +2223,9 @@
         <v>73</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="13"/>
@@ -2248,10 +2261,12 @@
       <c r="E16" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="11" t="s">
         <v>5</v>
@@ -2282,9 +2297,9 @@
         <v>80</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>94</v>
       </c>
       <c r="G17" s="13"/>
@@ -2320,9 +2335,9 @@
         <v>67</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="24" t="s">
         <v>93</v>
       </c>
       <c r="G18" s="9" t="s">
@@ -2358,9 +2373,9 @@
         <v>74</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>92</v>
       </c>
       <c r="G19" s="13"/>
@@ -2394,9 +2409,9 @@
         <v>75</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>92</v>
       </c>
       <c r="G20" s="9"/>
@@ -2431,9 +2446,9 @@
         <v>76</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="25" t="s">
         <v>100</v>
       </c>
       <c r="G21" s="13"/>
@@ -2464,13 +2479,13 @@
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="9" t="s">
         <v>119</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -8254,7 +8269,7 @@
     <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A362" s="7"/>
       <c r="B362" s="7" t="e">
-        <f t="shared" ref="B329:B392" si="6">LEFT(A362, FIND(".",A362)-1)</f>
+        <f t="shared" ref="B362:B392" si="6">LEFT(A362, FIND(".",A362)-1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C362" s="7"/>

</xml_diff>

<commit_message>
update sprint planning after first sprint planning meeting
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Moeri\Google Drive\BFH\20FS\SEaD\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F32984-AEC9-42A7-9333-DDD3DC553D2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE574A7-36A5-4D95-9263-63B0B6F709BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Available Ressources" sheetId="5" r:id="rId2"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId3"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId4"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
-    <sheet name="Status" sheetId="6" r:id="rId6"/>
+    <sheet name="Review" sheetId="7" r:id="rId5"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId6"/>
+    <sheet name="Status" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Status">Status!$A$1:$A$4</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
   <si>
     <t>ID</t>
   </si>
@@ -420,6 +421,24 @@
   </si>
   <si>
     <t>Set up page skeletons and a routing mechanism</t>
+  </si>
+  <si>
+    <t>very low</t>
+  </si>
+  <si>
+    <t>Sprint 1 per Person</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Ownership</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Planned Hours</t>
   </si>
 </sst>
 </file>
@@ -496,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -569,6 +588,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +936,7 @@
   <dimension ref="A1:BP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,12 +1088,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1162,8 @@
   <dimension ref="A1:DH12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1403,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="15">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F5" s="15">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A5,'Sprint Backlog'!K:K)</f>
@@ -1405,7 +1431,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A6,'Sprint Backlog'!K:K)</f>
@@ -1433,7 +1459,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="15">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A7,'Sprint Backlog'!K:K)</f>
@@ -1461,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="11">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F8" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A8,'Sprint Backlog'!K:K)</f>
@@ -1489,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="15">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F9" s="15">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A9,'Sprint Backlog'!K:K)</f>
@@ -1517,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="11">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F10" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A10,'Sprint Backlog'!K:K)</f>
@@ -1545,7 +1571,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="15">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F11" s="15">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A11,'Sprint Backlog'!K:K)</f>
@@ -1570,10 +1596,10 @@
         <v>55</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="E12" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F12" s="11">
         <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A12,'Sprint Backlog'!K:K)</f>
@@ -1602,8 +1628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CA444"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1774,9 @@
       <c r="G2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="I2" s="11" t="s">
         <v>5</v>
       </c>
@@ -1782,7 +1811,9 @@
       <c r="F3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="13" t="s">
         <v>35</v>
       </c>
@@ -1823,7 +1854,9 @@
       <c r="G4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1891,9 @@
       <c r="F5" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H5" s="13" t="s">
         <v>35</v>
       </c>
@@ -1899,7 +1934,9 @@
       <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="I6" s="11" t="s">
         <v>6</v>
       </c>
@@ -1934,8 +1971,12 @@
       <c r="F7" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="I7" s="15" t="s">
         <v>5</v>
       </c>
@@ -1970,8 +2011,12 @@
       <c r="F8" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="I8" s="23" t="s">
         <v>5</v>
       </c>
@@ -2006,8 +2051,12 @@
       <c r="F9" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="I9" s="15" t="s">
         <v>6</v>
       </c>
@@ -2042,8 +2091,12 @@
       <c r="F10" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="I10" s="11" t="s">
         <v>5</v>
       </c>
@@ -2081,7 +2134,9 @@
       <c r="G11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="I11" s="15" t="s">
         <v>5</v>
       </c>
@@ -2116,7 +2171,9 @@
       <c r="F12" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H12" s="9" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2214,9 @@
       <c r="G13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="I13" s="15" t="s">
         <v>6</v>
       </c>
@@ -2192,8 +2251,12 @@
       <c r="F14" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="I14" s="11" t="s">
         <v>5</v>
       </c>
@@ -2228,8 +2291,12 @@
       <c r="F15" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="15" t="s">
         <v>6</v>
       </c>
@@ -2267,7 +2334,9 @@
       <c r="G16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="I16" s="11" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2371,9 @@
       <c r="F17" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H17" s="13" t="s">
         <v>35</v>
       </c>
@@ -2343,7 +2414,9 @@
       <c r="G18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="I18" s="11" t="s">
         <v>6</v>
       </c>
@@ -2378,8 +2451,12 @@
       <c r="F19" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="G19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="I19" s="15" t="s">
         <v>6</v>
       </c>
@@ -2414,8 +2491,12 @@
       <c r="F20" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="G20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="I20" s="11" t="s">
         <v>6</v>
       </c>
@@ -2451,8 +2532,12 @@
       <c r="F21" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="G21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="I21" s="15" t="s">
         <v>7</v>
       </c>
@@ -2487,8 +2572,12 @@
       <c r="F22" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="I22" s="11" t="s">
         <v>7</v>
       </c>
@@ -9600,6 +9689,180 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C50E621-2136-4AD7-A410-32E3BCA06241}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="17">
+        <f>'Available Ressources'!$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="E3" s="17">
+        <f>SUMIF('Sprint Backlog'!G:G,Review!$C3,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+      <c r="F3" s="17">
+        <f>SUMIF('Sprint Backlog'!H:H,Review!$C3,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="17">
+        <f>'Available Ressources'!$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="E4" s="17">
+        <f>SUMIF('Sprint Backlog'!G:G,Review!$C4,'Sprint Backlog'!$J:$J)</f>
+        <v>5</v>
+      </c>
+      <c r="F4" s="17">
+        <f>SUMIF('Sprint Backlog'!H:H,Review!$C4,'Sprint Backlog'!$J:$J)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="17">
+        <f>'Available Ressources'!$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="17">
+        <f>SUMIF('Sprint Backlog'!G:G,Review!$C5,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="17">
+        <f>SUMIF('Sprint Backlog'!H:H,Review!$C5,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="17">
+        <f>'Available Ressources'!$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="E6" s="17">
+        <f>SUMIF('Sprint Backlog'!G:G,Review!$C6,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+      <c r="F6" s="17">
+        <f>SUMIF('Sprint Backlog'!H:H,Review!$C6,'Sprint Backlog'!$J:$J)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="17">
+        <f>'Available Ressources'!$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="E7" s="17">
+        <f>SUMIF('Sprint Backlog'!G:G,Review!$C7,'Sprint Backlog'!$J:$J)</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="17">
+        <f>SUMIF('Sprint Backlog'!H:H,Review!$C7,'Sprint Backlog'!$J:$J)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -9662,7 +9925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A0E942-7A01-4A0F-949D-52DFCE20B935}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
add product owners to sprint planning
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Moeri\Google Drive\BFH\20FS\SEaD\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE574A7-36A5-4D95-9263-63B0B6F709BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF85E6A2-B025-47DF-B764-4DB71E78C0B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -439,6 +439,36 @@
   </si>
   <si>
     <t>Planned Hours</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Künzler, Urs</t>
+  </si>
+  <si>
+    <t>Vogel, Jürgen</t>
+  </si>
+  <si>
+    <t>UrsKuenzler</t>
+  </si>
+  <si>
+    <t>vgj1</t>
+  </si>
+  <si>
+    <t>vj</t>
+  </si>
+  <si>
+    <t>ku</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
   </si>
 </sst>
 </file>
@@ -515,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -595,6 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP6"/>
+  <dimension ref="A1:BP8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,6 +975,7 @@
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" s="2" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -956,7 +988,9 @@
       <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1"/>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
@@ -1032,6 +1066,9 @@
       <c r="C2" s="17" t="s">
         <v>34</v>
       </c>
+      <c r="D2" s="29" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1043,6 +1080,9 @@
       <c r="C3" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="D3" s="18" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -1054,6 +1094,9 @@
       <c r="C4" s="17" t="s">
         <v>36</v>
       </c>
+      <c r="D4" s="29" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -1065,6 +1108,9 @@
       <c r="C5" s="18" t="s">
         <v>37</v>
       </c>
+      <c r="D5" s="18" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -1075,6 +1121,37 @@
       </c>
       <c r="C6" s="17" t="s">
         <v>38</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -9692,7 +9769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C50E621-2136-4AD7-A410-32E3BCA06241}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add first draft of sprint 2 backlog
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Moeri\Google Drive\BFH\20FS\SEaD\ch.bfh.bti7081.s2020.green\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\intelij-workspace\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EAA67B-2355-404A-B6D4-3C6F9ECC79F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242AD918-1BAE-4F2F-AAF3-6908A98EBEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Available Ressources" sheetId="5" r:id="rId2"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId3"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId4"/>
-    <sheet name="Review" sheetId="7" r:id="rId5"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId6"/>
-    <sheet name="Status" sheetId="6" r:id="rId7"/>
+    <sheet name="Sprint 1 Backlog" sheetId="2" r:id="rId4"/>
+    <sheet name="Sprint 2 Backlog" sheetId="8" r:id="rId5"/>
+    <sheet name="Review" sheetId="7" r:id="rId6"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId7"/>
+    <sheet name="Status" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint Backlog'!$A$1:$CA$443</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint 1 Backlog'!$A$1:$CA$443</definedName>
     <definedName name="Status">Status!$A$1:$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -30,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="202">
   <si>
     <t>ID</t>
   </si>
@@ -470,6 +473,180 @@
   </si>
   <si>
     <t>Product Owner</t>
+  </si>
+  <si>
+    <t>HealhtVisitor Model</t>
+  </si>
+  <si>
+    <t>Its possible to add notifications to a HealthVisitor</t>
+  </si>
+  <si>
+    <t>HealthVisitorManager</t>
+  </si>
+  <si>
+    <t>Add Notifications to HaealthClients on defined events</t>
+  </si>
+  <si>
+    <t>Trigger Notification events</t>
+  </si>
+  <si>
+    <t>Dashboard: View</t>
+  </si>
+  <si>
+    <t>Show dummy notifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: ShowNotifications </t>
+  </si>
+  <si>
+    <t>Protocolmanager, PersistenceManager</t>
+  </si>
+  <si>
+    <t>Changes of protocols in ProtocolManager are stored in database</t>
+  </si>
+  <si>
+    <t>Persistence:  UpdateProtocol</t>
+  </si>
+  <si>
+    <t>ProtocolManager</t>
+  </si>
+  <si>
+    <t>Methods to update an existsting protocol is available on ProtocolManager</t>
+  </si>
+  <si>
+    <t>Manager: UpdateProtocol</t>
+  </si>
+  <si>
+    <t>Protocol: View, Presenter</t>
+  </si>
+  <si>
+    <t>Ist possible to open an existing protocol in an edit view</t>
+  </si>
+  <si>
+    <t>View: EditProtcol</t>
+  </si>
+  <si>
+    <t>Protocolmanager</t>
+  </si>
+  <si>
+    <t>Implement filters on data layer for protocols</t>
+  </si>
+  <si>
+    <t>Manager:  ProtocolFilter</t>
+  </si>
+  <si>
+    <t>HealthClient: View, Presenter</t>
+  </si>
+  <si>
+    <t>Create view with input data to filter the protocol list</t>
+  </si>
+  <si>
+    <t>View: FilterProtocols</t>
+  </si>
+  <si>
+    <t>Its possible to load protocols per client</t>
+  </si>
+  <si>
+    <t>Manager: LoadProtocols per Client</t>
+  </si>
+  <si>
+    <t>Protocols of a given HealthClients are displayed on his profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: ProtocolHistory </t>
+  </si>
+  <si>
+    <t>Views with detailed data of a protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View: ProtocolDetail </t>
+  </si>
+  <si>
+    <t>View with all Protocols of specific HealthClient</t>
+  </si>
+  <si>
+    <t>View: ProtocolList</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Do task08</t>
+  </si>
+  <si>
+    <t>Document database connection</t>
+  </si>
+  <si>
+    <t>There is a solution to save and load protocols from the database</t>
+  </si>
+  <si>
+    <t>Initialize Persistencemanager</t>
+  </si>
+  <si>
+    <t>View with form to create a new protocol</t>
+  </si>
+  <si>
+    <t>View: CreateProtocol</t>
+  </si>
+  <si>
+    <t>Ist possible to view a single protocol</t>
+  </si>
+  <si>
+    <t>View: ShowProtocol</t>
+  </si>
+  <si>
+    <t>PersistenceManager</t>
+  </si>
+  <si>
+    <t>Implement loadProtocols from database and replace mock</t>
+  </si>
+  <si>
+    <t>Persistence: getProtocols</t>
+  </si>
+  <si>
+    <t>Create mock method to get Protocols from database</t>
+  </si>
+  <si>
+    <t>Mock Database getProtocols</t>
+  </si>
+  <si>
+    <t>Initialize Protocolmanager with data from PersistenceManager</t>
+  </si>
+  <si>
+    <t>Initialize Protocolmanager</t>
+  </si>
+  <si>
+    <t>Create a Test Set of at least  3 different Protocols per HealthClient</t>
+  </si>
+  <si>
+    <t>Create Protocol Test Set</t>
+  </si>
+  <si>
+    <t>Protocol: Model</t>
+  </si>
+  <si>
+    <t>Model for Protocol</t>
+  </si>
+  <si>
+    <t>Protocol Model</t>
+  </si>
+  <si>
+    <t>Implement loadAppointments from database and replace mock</t>
+  </si>
+  <si>
+    <t>Persistence: getAppointments</t>
+  </si>
+  <si>
+    <t>PersistenceManager: Test Data</t>
+  </si>
+  <si>
+    <t>Create mock method to get Appointments from database</t>
+  </si>
+  <si>
+    <t>Mock Database getAppointments</t>
+  </si>
+  <si>
+    <t>Add Notification-funtionality to HealthVisitor</t>
   </si>
 </sst>
 </file>
@@ -539,7 +716,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -562,11 +739,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -654,9 +842,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -672,7 +863,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -998,7 +1189,7 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -1196,7 +1387,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1286,7 +1477,7 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
@@ -1442,11 +1633,11 @@
         <v>16</v>
       </c>
       <c r="F2" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A2,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A2,'Sprint 1 Backlog'!K:K)</f>
         <v>16</v>
       </c>
       <c r="G2" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A2,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A2,'Sprint 1 Backlog'!L:L)</f>
         <v>14</v>
       </c>
       <c r="H2" s="10" t="s">
@@ -1470,11 +1661,11 @@
         <v>12</v>
       </c>
       <c r="F3" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A3,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A3,'Sprint 1 Backlog'!K:K)</f>
         <v>11</v>
       </c>
       <c r="G3" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A3,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A3,'Sprint 1 Backlog'!L:L)</f>
         <v>5</v>
       </c>
       <c r="H3" s="14" t="s">
@@ -1498,11 +1689,11 @@
         <v>12</v>
       </c>
       <c r="F4" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A4,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A4,'Sprint 1 Backlog'!K:K)</f>
         <v>11</v>
       </c>
       <c r="G4" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A4,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A4,'Sprint 1 Backlog'!L:L)</f>
         <v>4</v>
       </c>
       <c r="H4" s="10" t="s">
@@ -1526,11 +1717,11 @@
         <v>16</v>
       </c>
       <c r="F5" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A5,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A5,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G5" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A5,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A5,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H5" s="14" t="s">
@@ -1554,11 +1745,11 @@
         <v>8</v>
       </c>
       <c r="F6" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A6,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A6,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G6" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A6,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A6,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -1582,11 +1773,11 @@
         <v>16</v>
       </c>
       <c r="F7" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A7,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A7,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G7" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A7,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A7,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H7" s="14" t="s">
@@ -1610,11 +1801,11 @@
         <v>16</v>
       </c>
       <c r="F8" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A8,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A8,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G8" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A8,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A8,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H8" s="10" t="s">
@@ -1638,11 +1829,11 @@
         <v>12</v>
       </c>
       <c r="F9" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A9,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A9,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G9" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A9,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A9,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H9" s="14" t="s">
@@ -1666,11 +1857,11 @@
         <v>12</v>
       </c>
       <c r="F10" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A10,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A10,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G10" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A10,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A10,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H10" s="10" t="s">
@@ -1694,11 +1885,11 @@
         <v>12</v>
       </c>
       <c r="F11" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A11,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A11,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G11" s="14">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A11,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A11,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H11" s="14" t="s">
@@ -1722,11 +1913,11 @@
         <v>8</v>
       </c>
       <c r="F12" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A12,'Sprint Backlog'!K:K)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A12,'Sprint 1 Backlog'!K:K)</f>
         <v>0</v>
       </c>
       <c r="G12" s="10">
-        <f>SUMIF('Sprint Backlog'!B:B,'Product Backlog'!A12,'Sprint Backlog'!L:L)</f>
+        <f>SUMIF('Sprint 1 Backlog'!B:B,'Product Backlog'!A12,'Sprint 1 Backlog'!L:L)</f>
         <v>0</v>
       </c>
       <c r="H12" s="10" t="s">
@@ -1748,12 +1939,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CA444"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" hidden="1" customWidth="1"/>
@@ -9833,10 +10024,993 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB9057-DB96-4490-AA5C-2C8E1D8C4158}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2</v>
+      </c>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="10">
+        <v>4</v>
+      </c>
+      <c r="J5" s="10">
+        <v>4</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="10">
+        <v>2</v>
+      </c>
+      <c r="J7" s="10">
+        <v>2</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="10">
+        <v>2</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="10">
+        <v>3</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="10">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="10">
+        <v>4</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>4.8</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="10">
+        <v>4</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="10">
+        <v>2</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="10">
+        <v>2</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>5.2</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>5.3</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="10">
+        <v>2</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>5.4</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="10">
+        <v>2</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>6.1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="10">
+        <v>2</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="10">
+        <v>4</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>8.1</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="10">
+        <v>4</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="10">
+        <v>2</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="10">
+        <v>2</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="10">
+        <v>2</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>7.2</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="10">
+        <v>4</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>7.3</v>
+      </c>
+      <c r="B28" s="8">
+        <v>2</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="10">
+        <v>1</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8">
+        <v>2</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8">
+        <v>2</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8">
+        <v>2</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8">
+        <v>2</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L32" xr:uid="{06F441D2-3BEA-4D5B-BF28-5AD61F868919}">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -9844,7 +11018,7 @@
       <selection activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -9901,11 +11075,11 @@
         <v>8</v>
       </c>
       <c r="E3" s="16">
-        <f>SUMIF('Sprint Backlog'!G:G,Review!$C3,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!G:G,Review!$C3,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
       <c r="F3" s="16">
-        <f>SUMIF('Sprint Backlog'!H:H,Review!$C3,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!H:H,Review!$C3,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
     </row>
@@ -9924,11 +11098,11 @@
         <v>8</v>
       </c>
       <c r="E4" s="17">
-        <f>SUMIF('Sprint Backlog'!G:G,Review!$C4,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!G:G,Review!$C4,'Sprint 1 Backlog'!$J:$J)</f>
         <v>5</v>
       </c>
       <c r="F4" s="17">
-        <f>SUMIF('Sprint Backlog'!H:H,Review!$C4,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!H:H,Review!$C4,'Sprint 1 Backlog'!$J:$J)</f>
         <v>9</v>
       </c>
     </row>
@@ -9947,11 +11121,11 @@
         <v>8</v>
       </c>
       <c r="E5" s="16">
-        <f>SUMIF('Sprint Backlog'!G:G,Review!$C5,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!G:G,Review!$C5,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
       <c r="F5" s="16">
-        <f>SUMIF('Sprint Backlog'!H:H,Review!$C5,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!H:H,Review!$C5,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
     </row>
@@ -9970,11 +11144,11 @@
         <v>8</v>
       </c>
       <c r="E6" s="17">
-        <f>SUMIF('Sprint Backlog'!G:G,Review!$C6,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!G:G,Review!$C6,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
       <c r="F6" s="17">
-        <f>SUMIF('Sprint Backlog'!H:H,Review!$C6,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!H:H,Review!$C6,'Sprint 1 Backlog'!$J:$J)</f>
         <v>8</v>
       </c>
     </row>
@@ -9993,11 +11167,11 @@
         <v>8</v>
       </c>
       <c r="E7" s="16">
-        <f>SUMIF('Sprint Backlog'!G:G,Review!$C7,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!G:G,Review!$C7,'Sprint 1 Backlog'!$J:$J)</f>
         <v>9</v>
       </c>
       <c r="F7" s="16">
-        <f>SUMIF('Sprint Backlog'!H:H,Review!$C7,'Sprint Backlog'!$J:$J)</f>
+        <f>SUMIF('Sprint 1 Backlog'!H:H,Review!$C7,'Sprint 1 Backlog'!$J:$J)</f>
         <v>5</v>
       </c>
     </row>
@@ -10006,7 +11180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BF3"/>
   <sheetViews>
@@ -10014,7 +11188,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
@@ -10123,7 +11297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -10131,7 +11305,7 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Sprint 2 Backlog Done
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\intelij-workspace\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242AD918-1BAE-4F2F-AAF3-6908A98EBEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA044253-BC0F-4372-B8EB-D402FB7A5A04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>Add Notification-funtionality to HealthVisitor</t>
+  </si>
+  <si>
+    <t>Update classdiagram</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1477,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:H4"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10030,10 +10033,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB9057-DB96-4490-AA5C-2C8E1D8C4158}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10282,8 +10285,12 @@
       <c r="E7" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>7</v>
       </c>
@@ -10314,8 +10321,12 @@
       <c r="E8" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>5</v>
       </c>
@@ -10344,8 +10355,12 @@
       <c r="E9" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>6</v>
       </c>
@@ -10374,8 +10389,12 @@
       <c r="E10" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>5</v>
       </c>
@@ -10388,7 +10407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>4.4000000000000004</v>
       </c>
@@ -10402,10 +10421,14 @@
         <v>187</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+        <v>155</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H11" s="10" t="s">
         <v>5</v>
       </c>
@@ -10434,8 +10457,12 @@
       <c r="E12" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="10" t="s">
         <v>6</v>
       </c>
@@ -10464,8 +10491,12 @@
       <c r="E13" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="H13" s="10" t="s">
         <v>5</v>
       </c>
@@ -10494,8 +10525,12 @@
       <c r="E14" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="H14" s="10" t="s">
         <v>6</v>
       </c>
@@ -10509,7 +10544,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
+      <c r="A15" s="8">
         <v>4.8</v>
       </c>
       <c r="B15" s="8">
@@ -10524,8 +10559,12 @@
       <c r="E15" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H15" s="10" t="s">
         <v>5</v>
       </c>
@@ -10554,8 +10593,12 @@
       <c r="E16" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="10" t="s">
         <v>7</v>
       </c>
@@ -10584,8 +10627,12 @@
       <c r="E17" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H17" s="10" t="s">
         <v>6</v>
       </c>
@@ -10598,7 +10645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5.2</v>
       </c>
@@ -10614,8 +10661,12 @@
       <c r="E18" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="H18" s="10" t="s">
         <v>6</v>
       </c>
@@ -10644,8 +10695,12 @@
       <c r="E19" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H19" s="10" t="s">
         <v>6</v>
       </c>
@@ -10674,8 +10729,12 @@
       <c r="E20" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H20" s="10" t="s">
         <v>6</v>
       </c>
@@ -10688,7 +10747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>6.1</v>
       </c>
@@ -10704,8 +10763,12 @@
       <c r="E21" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H21" s="10" t="s">
         <v>6</v>
       </c>
@@ -10718,7 +10781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>6.2</v>
       </c>
@@ -10734,8 +10797,12 @@
       <c r="E22" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10764,8 +10831,12 @@
       <c r="E23" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="H23" s="10" t="s">
         <v>7</v>
       </c>
@@ -10778,7 +10849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>8.1999999999999993</v>
       </c>
@@ -10794,8 +10865,12 @@
       <c r="E24" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="H24" s="10" t="s">
         <v>7</v>
       </c>
@@ -10808,7 +10883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>8.3000000000000007</v>
       </c>
@@ -10824,8 +10899,12 @@
       <c r="E25" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="H25" s="10" t="s">
         <v>7</v>
       </c>
@@ -10868,7 +10947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>7.2</v>
       </c>
@@ -10898,7 +10977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>7.3</v>
       </c>
@@ -10933,80 +11012,37 @@
       <c r="B29" s="8">
         <v>2</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="8" t="s">
+        <v>202</v>
+      </c>
       <c r="D29" s="11"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
+      <c r="F29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="10">
+        <v>2</v>
+      </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8">
-        <v>2</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8">
-        <v>2</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8">
-        <v>2</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L32" xr:uid="{06F441D2-3BEA-4D5B-BF28-5AD61F868919}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L29" xr:uid="{06F441D2-3BEA-4D5B-BF28-5AD61F868919}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Sprint 3 Backlog
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\intelij-workspace\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC2C1E9-936F-4BE9-B55F-0E57FFBAE7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A9F10-0B4A-48E6-89CA-0C45544ED2B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Product Backlog" sheetId="1" r:id="rId3"/>
     <sheet name="Sprint 1 Backlog" sheetId="2" r:id="rId4"/>
     <sheet name="Sprint 2 Backlog" sheetId="8" r:id="rId5"/>
-    <sheet name="Review" sheetId="7" r:id="rId6"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId7"/>
-    <sheet name="Status" sheetId="6" r:id="rId8"/>
+    <sheet name="Sprint 3 Backlog" sheetId="9" r:id="rId6"/>
+    <sheet name="Review" sheetId="7" r:id="rId7"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId8"/>
+    <sheet name="Status" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint 1 Backlog'!$A$1:$CA$443</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -650,6 +651,87 @@
   </si>
   <si>
     <t>Update classdiagram</t>
+  </si>
+  <si>
+    <t>Static Code analyse</t>
+  </si>
+  <si>
+    <t>Run spotbugs</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Model: FAQ</t>
+  </si>
+  <si>
+    <t>Create FAQ Model</t>
+  </si>
+  <si>
+    <t>View: Show FAQ List</t>
+  </si>
+  <si>
+    <t>Manager: LoadFAQ</t>
+  </si>
+  <si>
+    <t>Ist possible to load FAQ Objects</t>
+  </si>
+  <si>
+    <t>ApplicationModelManager, PersistenceManager</t>
+  </si>
+  <si>
+    <t>View: FAQ Detail</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Cleanup</t>
+  </si>
+  <si>
+    <t>Manager: Multiuser</t>
+  </si>
+  <si>
+    <t>Move currentUser to Session</t>
+  </si>
+  <si>
+    <t>HealhtVisitor Manager</t>
+  </si>
+  <si>
+    <t>View all FAQs available</t>
+  </si>
+  <si>
+    <t>View details of an FAQ entry</t>
+  </si>
+  <si>
+    <t>Hilfe: View</t>
+  </si>
+  <si>
+    <t>Unify Layout</t>
+  </si>
+  <si>
+    <t>Show same layout on every page</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Model for Notifications</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Model: Notification</t>
+  </si>
+  <si>
+    <t>Describe dataprovider</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>Move config values to a single config file</t>
   </si>
 </sst>
 </file>
@@ -757,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -847,6 +929,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1387,7 +1472,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,11 +1558,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:DH12"/>
+  <dimension ref="A1:DH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,6 +2012,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="13" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H12" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -1943,8 +2046,8 @@
   <dimension ref="A1:CA444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P17" sqref="P17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10035,8 +10138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB9057-DB96-4490-AA5C-2C8E1D8C4158}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11130,6 +11233,598 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15B711E-0C6E-4B5A-9FBB-FC46A2BAD6F2}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="6"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="10">
+        <v>2</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>5.3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>5.4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>7.2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>7.3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>10.1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10.3</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="16">
+        <v>2</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10.4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="16">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12.1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="16">
+        <v>4</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12.2</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="16">
+        <v>4</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>12.3</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="16">
+        <v>2</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>12.4</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="16">
+        <v>2</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>12.5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="16">
+        <v>2</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L17" xr:uid="{AA051B77-EAC9-4B21-968E-19CEF353F35C}">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -11299,7 +11994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BF3"/>
   <sheetViews>
@@ -11416,7 +12111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Move profile image path to config & Update backlog
</commit_message>
<xml_diff>
--- a/doc/task06/team_green_scrum_planning.xlsx
+++ b/doc/task06/team_green_scrum_planning.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\intelij-workspace\ch.bfh.bti7081.s2020.green\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biasutti\IdeaProjects\ch.bfh.bti7081.s2020.green\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57980516-B38E-4756-A666-ADE9B8D747B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint 1 Backlog'!$A$1:$CA$443</definedName>
     <definedName name="Status">Status!$A$1:$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -752,7 +751,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1041,23 +1040,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1093,23 +1075,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1285,7 +1250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1483,7 +1448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1572,7 +1537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2048,7 +2013,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H12" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H12">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -2058,7 +2023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10139,9 +10104,9 @@
       <c r="M444" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CA443" xr:uid="{1058BA28-F955-4061-BB80-D8E922C7B585}"/>
+  <autoFilter ref="A1:CA443"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M238" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M238">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -10151,7 +10116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB9057-DB96-4490-AA5C-2C8E1D8C4158}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -11239,7 +11204,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L29" xr:uid="{06F441D2-3BEA-4D5B-BF28-5AD61F868919}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L29">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -11249,11 +11214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15B711E-0C6E-4B5A-9FBB-FC46A2BAD6F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11441,10 +11406,14 @@
       <c r="I5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
       <c r="L5" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -11475,10 +11444,14 @@
       <c r="I6" s="10">
         <v>2</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="10">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1</v>
+      </c>
       <c r="L6" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -11509,10 +11482,14 @@
       <c r="I7" s="10">
         <v>4</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="J7" s="10">
+        <v>4</v>
+      </c>
+      <c r="K7" s="10">
+        <v>4</v>
+      </c>
       <c r="L7" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -11543,10 +11520,14 @@
       <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="J8" s="10">
+        <v>2</v>
+      </c>
+      <c r="K8" s="10">
+        <v>2</v>
+      </c>
       <c r="L8" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -11979,7 +11960,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L17" xr:uid="{AA051B77-EAC9-4B21-968E-19CEF353F35C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L17">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -11989,7 +11970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12159,7 +12140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12276,7 +12257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>